<commit_message>
updates to link log
</commit_message>
<xml_diff>
--- a/extra_data/link_log.xlsx
+++ b/extra_data/link_log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jessica.dyer@leveltenenergy.com/Repositories/gbv-health-provider-study/extra_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{7CC82A52-EF74-8149-8AAB-4DB582724A6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{E0C449D9-ECA8-C84B-9778-B2A8E643E0FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10860" yWindow="500" windowWidth="28040" windowHeight="16400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="linklog" sheetId="1" r:id="rId1"/>
@@ -4039,8 +4039,8 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D677"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A642" workbookViewId="0">
-      <selection activeCell="C678" sqref="C678"/>
+    <sheetView tabSelected="1" topLeftCell="A533" workbookViewId="0">
+      <selection activeCell="F557" sqref="F557"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4129,7 +4129,7 @@
         <v>766</v>
       </c>
       <c r="C6">
-        <v>3</v>
+        <v>149</v>
       </c>
       <c r="D6">
         <v>3</v>
@@ -5585,7 +5585,7 @@
         <v>933</v>
       </c>
       <c r="C110">
-        <v>66</v>
+        <v>450</v>
       </c>
       <c r="D110">
         <v>3</v>
@@ -6047,7 +6047,7 @@
         <v>965</v>
       </c>
       <c r="C143">
-        <v>82</v>
+        <v>451</v>
       </c>
       <c r="D143">
         <v>3</v>
@@ -6285,7 +6285,7 @@
         <v>700</v>
       </c>
       <c r="C160">
-        <v>91</v>
+        <v>452</v>
       </c>
       <c r="D160">
         <v>3</v>

</xml_diff>

<commit_message>
remaining changes so i can move to attendance issues
</commit_message>
<xml_diff>
--- a/extra_data/link_log.xlsx
+++ b/extra_data/link_log.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/susanglenn/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/susanglenn/Repositories/gbv-health-provider-study/extra_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B711B0F1-F722-9646-B85C-DC32A9B000AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{9428B995-4111-BF4C-9DCB-F753D6DC090B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20640" yWindow="-740" windowWidth="20640" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-26420" yWindow="500" windowWidth="26420" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="import" sheetId="1" r:id="rId1"/>
@@ -3990,9 +3990,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://purl.oclc.org/ooxml/drawingml/main" name="Office Theme">
+<a:theme xmlns:a="http://purl.oclc.org/ooxml/drawingml/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -4030,7 +4030,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -4136,7 +4136,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -4278,7 +4278,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -4288,8 +4288,8 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K677"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A643" workbookViewId="0">
-      <selection activeCell="A670" sqref="A670:XFD670"/>
+    <sheetView tabSelected="1" topLeftCell="A291" workbookViewId="0">
+      <selection activeCell="B309" sqref="B309"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>